<commit_message>
Update.gitignore .DS_Store，Add  code/gym_exercises into main，Update progress report excel
</commit_message>
<xml_diff>
--- a/doc/Iteration3/CS673_ProgressReport_team6_iter3.xlsx
+++ b/doc/Iteration3/CS673_ProgressReport_team6_iter3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="356">
   <si>
     <t xml:space="preserve">This report has 1 group iteration progress summary sheet to be filled at the end of each iteration by the team leader, 
 1 project ontribution sheet to be filled by everyone at the end of the semester, and 1 weekly report sheet per student. </t>
@@ -1807,6 +1807,48 @@
     <t>0-Finshing Youtube Api and exercises Deatil Pages</t>
   </si>
   <si>
+    <t xml:space="preserve">0 - Learn Vue , Cypress. 
+1 - define new feature netlify deployment
+2 - design profile card css
+4 - design exercises detail page
+5 - Taking Part in Group Meeting </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Finishing profile card css 
+2. finishing exercises detail page UI font
+</t>
+  </si>
+  <si>
+    <t>0-Finshing Youtube Api and 
+exercises Deatil Pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 - Learn React, Vue, Cypress
+1 - Design and try Youtube API
+2 - debugging api functons. 
+4 - Test youtube api for exercise detail page. 
+5 - Taking Part in the group meeting
+</t>
+  </si>
+  <si>
+    <t>1. Finishing youtube Api testing</t>
+  </si>
+  <si>
+    <t>Thanks Giving week</t>
+  </si>
+  <si>
+    <t>1 - Design Exercise Detail Page UI
+2 -  Design Youtube API Intergratation
+3 - Splitting Demo with User Story and Updating Jira 
+4 - Testing all functions in Exercise Detail Page
+6 - Deploy the Video Illustaion Page on Netlify
+7- Creating PPT for requirement analysis</t>
+  </si>
+  <si>
+    <t>1. Finishing Requiremnt Analysis PPT
+2. Finishing Deployment Video and Illustration Part</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <rFont val="Arial"/>
@@ -1856,7 +1898,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1890,6 +1932,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1932,7 +1978,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2047,6 +2093,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -31231,7 +31283,7 @@
         <v>323</v>
       </c>
       <c r="S6" s="8">
-        <f t="shared" ref="S6:S11" si="1">G6+H6+I6+J6+K6+L6+M6+N6</f>
+        <f t="shared" ref="S6:S23" si="1">G6+H6+I6+J6+K6+L6+M6+N6</f>
         <v>11.7</v>
       </c>
       <c r="T6" s="8"/>
@@ -31552,60 +31604,143 @@
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
     </row>
-    <row r="12" ht="58.5" customHeight="1">
+    <row r="12" ht="120.0" customHeight="1">
       <c r="A12" s="24">
         <v>9.0</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>290</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
+      <c r="C12" s="8">
+        <f t="shared" ref="C12:C13" si="3">D12+E12</f>
+        <v>6.5</v>
+      </c>
+      <c r="D12" s="8">
+        <f t="shared" ref="D12:D15" si="4">sum(G12:N12)</f>
+        <v>5.5</v>
+      </c>
+      <c r="E12" s="24">
+        <v>1.0</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>341</v>
+      </c>
+      <c r="G12" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="H12" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="I12" s="10">
+        <v>1.0</v>
+      </c>
       <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
+      <c r="K12" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="L12" s="10">
+        <v>1.5</v>
+      </c>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
+      <c r="O12" s="41" t="s">
+        <v>342</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="R12" s="42" t="s">
+        <v>343</v>
+      </c>
+      <c r="S12" s="8">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
       <c r="T12" s="8"/>
       <c r="U12" s="8"/>
       <c r="V12" s="8"/>
     </row>
-    <row r="13" ht="38.25" customHeight="1">
+    <row r="13" ht="91.5" customHeight="1">
       <c r="A13" s="24">
         <v>10.0</v>
       </c>
       <c r="B13" s="24" t="s">
         <v>296</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
+      <c r="C13" s="8">
+        <f t="shared" si="3"/>
+        <v>6.5</v>
+      </c>
+      <c r="D13" s="8">
+        <f t="shared" si="4"/>
+        <v>5.5</v>
+      </c>
+      <c r="E13" s="24">
+        <v>1.0</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>344</v>
+      </c>
+      <c r="G13" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="H13" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="I13" s="10">
+        <v>1.0</v>
+      </c>
       <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
+      <c r="K13" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="L13" s="10">
+        <v>1.5</v>
+      </c>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
+      <c r="O13" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="P13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="R13" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="S13" s="8">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
       <c r="T13" s="8"/>
       <c r="U13" s="8"/>
       <c r="V13" s="8"/>
     </row>
-    <row r="14" ht="48.0" customHeight="1">
+    <row r="14" ht="85.5" customHeight="1">
       <c r="A14" s="24">
         <v>11.0</v>
       </c>
       <c r="B14" s="24" t="s">
         <v>302</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="D14" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>346</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -31619,31 +31754,71 @@
       <c r="P14" s="8"/>
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
+      <c r="S14" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="T14" s="8"/>
       <c r="U14" s="8"/>
       <c r="V14" s="8"/>
     </row>
-    <row r="15" ht="48.0" customHeight="1">
+    <row r="15" ht="96.0" customHeight="1">
       <c r="A15" s="24">
         <v>12.0</v>
       </c>
       <c r="B15" s="24" t="s">
         <v>308</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
+      <c r="C15" s="8">
+        <f>D15+E15</f>
+        <v>7.5</v>
+      </c>
+      <c r="D15" s="8">
+        <f t="shared" si="4"/>
+        <v>5.5</v>
+      </c>
+      <c r="E15" s="24">
+        <v>2.0</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>347</v>
+      </c>
+      <c r="G15" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="H15" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="I15" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="J15" s="10">
+        <v>1.0</v>
+      </c>
       <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
+      <c r="L15" s="10">
+        <v>0.5</v>
+      </c>
       <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
+      <c r="N15" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q15" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="R15" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="S15" s="8">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
       <c r="T15" s="8"/>
       <c r="U15" s="8"/>
       <c r="V15" s="8"/>
@@ -31661,7 +31836,10 @@
       <c r="P16" s="8"/>
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
+      <c r="S16" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="T16" s="8"/>
       <c r="U16" s="8"/>
       <c r="V16" s="8"/>
@@ -31679,7 +31857,10 @@
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
+      <c r="S17" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="T17" s="8"/>
       <c r="U17" s="8"/>
       <c r="V17" s="8"/>
@@ -31697,7 +31878,10 @@
       <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
+      <c r="S18" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="T18" s="8"/>
       <c r="U18" s="8"/>
       <c r="V18" s="8"/>
@@ -31715,7 +31899,10 @@
       <c r="P19" s="8"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
+      <c r="S19" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="T19" s="8"/>
       <c r="U19" s="8"/>
       <c r="V19" s="8"/>
@@ -31733,7 +31920,10 @@
       <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
+      <c r="S20" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="T20" s="8"/>
       <c r="U20" s="8"/>
       <c r="V20" s="8"/>
@@ -31751,7 +31941,10 @@
       <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
-      <c r="S21" s="8"/>
+      <c r="S21" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="T21" s="8"/>
       <c r="U21" s="8"/>
       <c r="V21" s="8"/>
@@ -31769,7 +31962,10 @@
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
+      <c r="S22" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="T22" s="8"/>
       <c r="U22" s="8"/>
       <c r="V22" s="8"/>
@@ -31787,7 +31983,10 @@
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
+      <c r="S23" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="T23" s="8"/>
       <c r="U23" s="8"/>
       <c r="V23" s="8"/>
@@ -36167,7 +36366,7 @@
     </row>
     <row r="2" ht="39.75" customHeight="1">
       <c r="A2" s="22" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -36257,7 +36456,7 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="C4" s="36">
         <f>D4+E4</f>
@@ -36271,7 +36470,7 @@
         <v>1.0</v>
       </c>
       <c r="F4" s="36" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="G4" s="36">
         <v>3.0</v>
@@ -36292,16 +36491,16 @@
         <v>0.5</v>
       </c>
       <c r="O4" s="36" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="P4" s="36" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
       <c r="Q4" s="36" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="R4" s="36" t="s">
-        <v>347</v>
+        <v>355</v>
       </c>
       <c r="S4" s="36">
         <v>6.0</v>

</xml_diff>